<commit_message>
Fix/rapidpro prop reminders (#185)
* fix: unmute expression

* fix: use reminders as RP prop

* fix: validation for country code
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/enroll.xlsx
+++ b/itech-malawi/forms/app/enroll.xlsx
@@ -252,7 +252,7 @@
     <t>../language_preference</t>
   </si>
   <si>
-    <t>reminder</t>
+    <t>reminders</t>
   </si>
   <si>
     <t>true</t>
@@ -318,7 +318,7 @@
     <t>Client's Mobile phone number</t>
   </si>
   <si>
-    <t xml:space="preserve">regex(., ‘^\+26[0-9]{9}$') </t>
+    <t xml:space="preserve">regex(., ‘^\+265[0-9]{9}$’) </t>
   </si>
   <si>
     <t>Please enter a valid mobile number</t>

</xml_diff>

<commit_message>
Feat/enrollment form lang code/187 (#188)
* fix: unmute expression

* feat: use ISO code for chichewa
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/enroll.xlsx
+++ b/itech-malawi/forms/app/enroll.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
   <si>
     <t>type</t>
   </si>
@@ -174,12 +174,6 @@
     <t>../person/phone</t>
   </si>
   <si>
-    <t>language_preference</t>
-  </si>
-  <si>
-    <t>../person/language_preference</t>
-  </si>
-  <si>
     <t>ctx</t>
   </si>
   <si>
@@ -243,10 +237,16 @@
     <t>optout</t>
   </si>
   <si>
+    <t>Optout</t>
+  </si>
+  <si>
     <t>false</t>
   </si>
   <si>
     <t>language</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language </t>
   </si>
   <si>
     <t>../language_preference</t>
@@ -255,13 +255,22 @@
     <t>reminders</t>
   </si>
   <si>
+    <t>Reminders</t>
+  </si>
+  <si>
     <t>true</t>
   </si>
   <si>
     <t>adherence</t>
   </si>
   <si>
+    <t>Adherence</t>
+  </si>
+  <si>
     <t>visit_date</t>
+  </si>
+  <si>
+    <t>Visit Date</t>
   </si>
   <si>
     <t>now()</t>
@@ -339,10 +348,22 @@
     <t>select_one language_preference</t>
   </si>
   <si>
+    <t>language_preference</t>
+  </si>
+  <si>
     <t>What is this client’s language of preference for the texts?</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>language_code</t>
+  </si>
+  <si>
+    <t>Language Code</t>
+  </si>
+  <si>
+    <t>if(selected(${language_preference}, ’english’), ‘eng’, ‘nya’)</t>
   </si>
   <si>
     <t>list_name</t>
@@ -2131,7 +2152,7 @@
     <col min="9" max="9" width="30.3516" style="1" customWidth="1"/>
     <col min="10" max="10" width="27.3516" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="36" style="1" customWidth="1"/>
+    <col min="12" max="12" width="49.5859" style="1" customWidth="1"/>
     <col min="13" max="13" width="17.8516" style="1" customWidth="1"/>
     <col min="14" max="14" width="20.8516" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.8516" style="1" customWidth="1"/>
@@ -2839,13 +2860,9 @@
       <c r="Z19" s="15"/>
       <c r="AA19" s="15"/>
     </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" t="s" s="30">
-        <v>44</v>
-      </c>
-      <c r="B20" t="s" s="31">
-        <v>53</v>
-      </c>
+    <row r="20" ht="15.75" customHeight="1">
+      <c r="A20" s="37"/>
+      <c r="B20" s="38"/>
       <c r="C20" s="32"/>
       <c r="D20" s="33"/>
       <c r="E20" s="34"/>
@@ -2855,9 +2872,7 @@
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
       <c r="K20" s="34"/>
-      <c r="L20" t="s" s="35">
-        <v>54</v>
-      </c>
+      <c r="L20" s="33"/>
       <c r="M20" s="34"/>
       <c r="N20" s="34"/>
       <c r="O20" s="34"/>
@@ -2874,23 +2889,23 @@
       <c r="Z20" s="15"/>
       <c r="AA20" s="15"/>
     </row>
-    <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="37"/>
-      <c r="B21" s="38"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="14"/>
+    <row r="21" ht="12.75" customHeight="1">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="29"/>
+      <c r="M21" s="27"/>
+      <c r="N21" s="27"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="15"/>
       <c r="Q21" s="15"/>
       <c r="R21" s="15"/>
       <c r="S21" s="15"/>
@@ -2904,22 +2919,28 @@
       <c r="AA21" s="15"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="27"/>
-      <c r="B22" s="27"/>
-      <c r="C22" s="28"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="27"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="28"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="15"/>
+      <c r="A22" t="s" s="39">
+        <v>44</v>
+      </c>
+      <c r="B22" t="s" s="40">
+        <v>53</v>
+      </c>
+      <c r="C22" s="41"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="42"/>
+      <c r="L22" t="s" s="44">
+        <v>54</v>
+      </c>
+      <c r="M22" s="43"/>
+      <c r="N22" s="43"/>
+      <c r="O22" s="43"/>
+      <c r="P22" s="14"/>
       <c r="Q22" s="15"/>
       <c r="R22" s="15"/>
       <c r="S22" s="15"/>
@@ -2969,23 +2990,27 @@
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" t="s" s="39">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s" s="40">
         <v>57</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="43"/>
+      <c r="C24" t="s" s="45">
+        <v>42</v>
+      </c>
+      <c r="D24" t="s" s="46">
+        <v>58</v>
+      </c>
+      <c r="E24" t="s" s="44">
+        <v>19</v>
+      </c>
       <c r="F24" s="43"/>
       <c r="G24" s="41"/>
       <c r="H24" s="43"/>
       <c r="I24" s="41"/>
       <c r="J24" s="41"/>
       <c r="K24" s="42"/>
-      <c r="L24" t="s" s="44">
-        <v>58</v>
-      </c>
+      <c r="L24" s="43"/>
       <c r="M24" s="43"/>
       <c r="N24" s="43"/>
       <c r="O24" s="43"/>
@@ -3004,20 +3029,16 @@
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" t="s" s="39">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="B25" t="s" s="40">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C25" t="s" s="45">
-        <v>42</v>
+        <v>61</v>
       </c>
-      <c r="D25" t="s" s="46">
-        <v>60</v>
-      </c>
-      <c r="E25" t="s" s="44">
-        <v>19</v>
-      </c>
+      <c r="D25" s="42"/>
+      <c r="E25" s="43"/>
       <c r="F25" s="43"/>
       <c r="G25" s="41"/>
       <c r="H25" s="43"/>
@@ -3043,22 +3064,28 @@
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" t="s" s="39">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" t="s" s="40">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C26" t="s" s="45">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="D26" s="42"/>
-      <c r="E26" s="43"/>
+      <c r="E26" t="s" s="44">
+        <v>23</v>
+      </c>
       <c r="F26" s="43"/>
       <c r="G26" s="41"/>
-      <c r="H26" s="43"/>
+      <c r="H26" t="s" s="45">
+        <v>64</v>
+      </c>
       <c r="I26" s="41"/>
       <c r="J26" s="41"/>
-      <c r="K26" s="42"/>
+      <c r="K26" s="47">
+        <v>0</v>
+      </c>
       <c r="L26" s="43"/>
       <c r="M26" s="43"/>
       <c r="N26" s="43"/>
@@ -3078,29 +3105,19 @@
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" t="s" s="39">
-        <v>64</v>
+        <v>43</v>
       </c>
-      <c r="B27" t="s" s="40">
-        <v>65</v>
-      </c>
-      <c r="C27" t="s" s="45">
-        <v>42</v>
-      </c>
+      <c r="B27" s="48"/>
+      <c r="C27" s="41"/>
       <c r="D27" s="42"/>
-      <c r="E27" t="s" s="44">
-        <v>23</v>
-      </c>
+      <c r="E27" s="43"/>
       <c r="F27" s="43"/>
       <c r="G27" s="41"/>
-      <c r="H27" t="s" s="45">
-        <v>66</v>
-      </c>
+      <c r="H27" s="43"/>
       <c r="I27" s="41"/>
       <c r="J27" s="41"/>
-      <c r="K27" s="47">
-        <v>0</v>
-      </c>
-      <c r="L27" s="43"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="42"/>
       <c r="M27" s="43"/>
       <c r="N27" s="43"/>
       <c r="O27" s="43"/>
@@ -3118,24 +3135,22 @@
       <c r="AA27" s="15"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" t="s" s="39">
-        <v>43</v>
-      </c>
-      <c r="B28" s="48"/>
-      <c r="C28" s="41"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="41"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="41"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="43"/>
-      <c r="L28" s="42"/>
-      <c r="M28" s="43"/>
-      <c r="N28" s="43"/>
-      <c r="O28" s="43"/>
-      <c r="P28" s="14"/>
+      <c r="A28" s="27"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="28"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="28"/>
+      <c r="J28" s="28"/>
+      <c r="K28" s="27"/>
+      <c r="L28" s="29"/>
+      <c r="M28" s="27"/>
+      <c r="N28" s="27"/>
+      <c r="O28" s="27"/>
+      <c r="P28" s="15"/>
       <c r="Q28" s="15"/>
       <c r="R28" s="15"/>
       <c r="S28" s="15"/>
@@ -3148,23 +3163,33 @@
       <c r="Z28" s="15"/>
       <c r="AA28" s="15"/>
     </row>
-    <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="27"/>
-      <c r="B29" s="27"/>
-      <c r="C29" s="28"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="15"/>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" t="s" s="49">
+        <v>15</v>
+      </c>
+      <c r="B29" t="s" s="50">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s" s="51">
+        <v>42</v>
+      </c>
+      <c r="D29" s="52"/>
+      <c r="E29" t="s" s="53">
+        <v>19</v>
+      </c>
+      <c r="F29" s="54"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="54"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
+      <c r="K29" s="54"/>
+      <c r="L29" s="52"/>
+      <c r="M29" t="s" s="53">
+        <v>65</v>
+      </c>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="14"/>
       <c r="Q29" s="15"/>
       <c r="R29" s="15"/>
       <c r="S29" s="15"/>
@@ -3178,31 +3203,29 @@
       <c r="AA29" s="15"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" t="s" s="49">
+      <c r="A30" t="s" s="56">
         <v>15</v>
       </c>
-      <c r="B30" t="s" s="50">
-        <v>48</v>
+      <c r="B30" t="s" s="57">
+        <v>40</v>
       </c>
-      <c r="C30" t="s" s="51">
+      <c r="C30" t="s" s="58">
         <v>42</v>
       </c>
-      <c r="D30" s="52"/>
-      <c r="E30" t="s" s="53">
-        <v>19</v>
+      <c r="D30" s="59"/>
+      <c r="E30" t="s" s="60">
+        <v>23</v>
       </c>
-      <c r="F30" s="54"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="55"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="54"/>
-      <c r="L30" s="52"/>
-      <c r="M30" t="s" s="53">
-        <v>67</v>
-      </c>
-      <c r="N30" s="54"/>
-      <c r="O30" s="54"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="62"/>
+      <c r="K30" s="61"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="61"/>
+      <c r="N30" s="61"/>
+      <c r="O30" s="61"/>
       <c r="P30" s="14"/>
       <c r="Q30" s="15"/>
       <c r="R30" s="15"/>
@@ -3218,10 +3241,10 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" t="s" s="56">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B31" t="s" s="57">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s" s="58">
         <v>42</v>
@@ -3236,7 +3259,9 @@
       <c r="I31" s="62"/>
       <c r="J31" s="62"/>
       <c r="K31" s="61"/>
-      <c r="L31" s="59"/>
+      <c r="L31" t="s" s="63">
+        <v>66</v>
+      </c>
       <c r="M31" s="61"/>
       <c r="N31" s="61"/>
       <c r="O31" s="61"/>
@@ -3255,17 +3280,17 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" t="s" s="56">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B32" t="s" s="57">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s" s="58">
         <v>42</v>
       </c>
       <c r="D32" s="59"/>
       <c r="E32" t="s" s="60">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F32" s="61"/>
       <c r="G32" s="62"/>
@@ -3273,9 +3298,7 @@
       <c r="I32" s="62"/>
       <c r="J32" s="62"/>
       <c r="K32" s="61"/>
-      <c r="L32" t="s" s="63">
-        <v>68</v>
-      </c>
+      <c r="L32" s="59"/>
       <c r="M32" s="61"/>
       <c r="N32" s="61"/>
       <c r="O32" s="61"/>
@@ -3294,17 +3317,17 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" t="s" s="56">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s" s="57">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s" s="58">
         <v>42</v>
       </c>
       <c r="D33" s="59"/>
       <c r="E33" t="s" s="60">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="F33" s="61"/>
       <c r="G33" s="62"/>
@@ -3312,7 +3335,9 @@
       <c r="I33" s="62"/>
       <c r="J33" s="62"/>
       <c r="K33" s="61"/>
-      <c r="L33" s="59"/>
+      <c r="L33" t="s" s="63">
+        <v>67</v>
+      </c>
       <c r="M33" s="61"/>
       <c r="N33" s="61"/>
       <c r="O33" s="61"/>
@@ -3329,29 +3354,21 @@
       <c r="Z33" s="15"/>
       <c r="AA33" s="15"/>
     </row>
-    <row r="34" ht="15.75" customHeight="1">
+    <row r="34" ht="12.75" customHeight="1">
       <c r="A34" t="s" s="56">
-        <v>44</v>
+        <v>43</v>
       </c>
-      <c r="B34" t="s" s="57">
-        <v>32</v>
-      </c>
-      <c r="C34" t="s" s="58">
-        <v>42</v>
-      </c>
+      <c r="B34" s="64"/>
+      <c r="C34" s="62"/>
       <c r="D34" s="59"/>
-      <c r="E34" t="s" s="60">
-        <v>23</v>
-      </c>
+      <c r="E34" s="61"/>
       <c r="F34" s="61"/>
       <c r="G34" s="62"/>
       <c r="H34" s="61"/>
       <c r="I34" s="62"/>
       <c r="J34" s="62"/>
       <c r="K34" s="61"/>
-      <c r="L34" t="s" s="63">
-        <v>69</v>
-      </c>
+      <c r="L34" s="59"/>
       <c r="M34" s="61"/>
       <c r="N34" s="61"/>
       <c r="O34" s="61"/>
@@ -3399,24 +3416,30 @@
       <c r="Z35" s="15"/>
       <c r="AA35" s="15"/>
     </row>
-    <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" t="s" s="56">
-        <v>43</v>
+    <row r="36" ht="15.75" customHeight="1">
+      <c r="A36" t="s" s="65">
+        <v>44</v>
       </c>
-      <c r="B36" s="64"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="61"/>
-      <c r="F36" s="61"/>
-      <c r="G36" s="62"/>
-      <c r="H36" s="61"/>
-      <c r="I36" s="62"/>
-      <c r="J36" s="62"/>
-      <c r="K36" s="61"/>
-      <c r="L36" s="59"/>
-      <c r="M36" s="61"/>
-      <c r="N36" s="61"/>
-      <c r="O36" s="61"/>
+      <c r="B36" t="s" s="53">
+        <v>0</v>
+      </c>
+      <c r="C36" t="s" s="66">
+        <v>68</v>
+      </c>
+      <c r="D36" s="67"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="68"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="68"/>
+      <c r="J36" s="68"/>
+      <c r="K36" s="64"/>
+      <c r="L36" t="s" s="69">
+        <v>69</v>
+      </c>
+      <c r="M36" s="64"/>
+      <c r="N36" s="64"/>
+      <c r="O36" s="64"/>
       <c r="P36" s="14"/>
       <c r="Q36" s="15"/>
       <c r="R36" s="15"/>
@@ -3435,11 +3458,9 @@
         <v>44</v>
       </c>
       <c r="B37" t="s" s="53">
-        <v>0</v>
-      </c>
-      <c r="C37" t="s" s="66">
         <v>70</v>
       </c>
+      <c r="C37" s="68"/>
       <c r="D37" s="67"/>
       <c r="E37" s="64"/>
       <c r="F37" s="64"/>
@@ -3469,23 +3490,23 @@
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s" s="65">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="B38" t="s" s="53">
         <v>72</v>
       </c>
       <c r="C38" s="68"/>
       <c r="D38" s="67"/>
-      <c r="E38" s="64"/>
+      <c r="E38" t="s" s="57">
+        <v>23</v>
+      </c>
       <c r="F38" s="64"/>
       <c r="G38" s="68"/>
       <c r="H38" s="64"/>
       <c r="I38" s="68"/>
       <c r="J38" s="68"/>
       <c r="K38" s="64"/>
-      <c r="L38" t="s" s="69">
-        <v>73</v>
-      </c>
+      <c r="L38" s="69"/>
       <c r="M38" s="64"/>
       <c r="N38" s="64"/>
       <c r="O38" s="64"/>
@@ -3504,23 +3525,25 @@
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s" s="65">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B39" t="s" s="53">
+        <v>73</v>
+      </c>
+      <c r="C39" t="s" s="66">
         <v>74</v>
       </c>
-      <c r="C39" s="68"/>
       <c r="D39" s="67"/>
-      <c r="E39" t="s" s="57">
-        <v>23</v>
-      </c>
+      <c r="E39" s="64"/>
       <c r="F39" s="64"/>
       <c r="G39" s="68"/>
       <c r="H39" s="64"/>
       <c r="I39" s="68"/>
       <c r="J39" s="68"/>
       <c r="K39" s="64"/>
-      <c r="L39" s="69"/>
+      <c r="L39" t="s" s="69">
+        <v>75</v>
+      </c>
       <c r="M39" s="64"/>
       <c r="N39" s="64"/>
       <c r="O39" s="64"/>
@@ -3542,9 +3565,11 @@
         <v>20</v>
       </c>
       <c r="B40" t="s" s="53">
-        <v>75</v>
+        <v>76</v>
       </c>
-      <c r="C40" s="68"/>
+      <c r="C40" t="s" s="66">
+        <v>77</v>
+      </c>
       <c r="D40" s="67"/>
       <c r="E40" s="64"/>
       <c r="F40" s="64"/>
@@ -3554,7 +3579,7 @@
       <c r="J40" s="68"/>
       <c r="K40" s="64"/>
       <c r="L40" t="s" s="69">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="M40" s="64"/>
       <c r="N40" s="64"/>
@@ -3577,9 +3602,11 @@
         <v>20</v>
       </c>
       <c r="B41" t="s" s="53">
-        <v>77</v>
+        <v>79</v>
       </c>
-      <c r="C41" s="68"/>
+      <c r="C41" t="s" s="66">
+        <v>80</v>
+      </c>
       <c r="D41" s="67"/>
       <c r="E41" s="64"/>
       <c r="F41" s="64"/>
@@ -3589,7 +3616,7 @@
       <c r="J41" s="68"/>
       <c r="K41" s="64"/>
       <c r="L41" t="s" s="69">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="M41" s="64"/>
       <c r="N41" s="64"/>
@@ -3612,9 +3639,11 @@
         <v>20</v>
       </c>
       <c r="B42" t="s" s="53">
-        <v>79</v>
+        <v>82</v>
       </c>
-      <c r="C42" s="68"/>
+      <c r="C42" t="s" s="66">
+        <v>83</v>
+      </c>
       <c r="D42" s="67"/>
       <c r="E42" s="64"/>
       <c r="F42" s="64"/>
@@ -3624,7 +3653,7 @@
       <c r="J42" s="68"/>
       <c r="K42" s="64"/>
       <c r="L42" t="s" s="69">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="M42" s="64"/>
       <c r="N42" s="64"/>
@@ -3647,9 +3676,11 @@
         <v>20</v>
       </c>
       <c r="B43" t="s" s="53">
-        <v>81</v>
+        <v>84</v>
       </c>
-      <c r="C43" s="68"/>
+      <c r="C43" t="s" s="66">
+        <v>85</v>
+      </c>
       <c r="D43" s="67"/>
       <c r="E43" s="64"/>
       <c r="F43" s="64"/>
@@ -3659,7 +3690,7 @@
       <c r="J43" s="68"/>
       <c r="K43" s="64"/>
       <c r="L43" t="s" s="69">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="M43" s="64"/>
       <c r="N43" s="64"/>
@@ -3679,11 +3710,9 @@
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" t="s" s="65">
-        <v>20</v>
+        <v>43</v>
       </c>
-      <c r="B44" t="s" s="53">
-        <v>82</v>
-      </c>
+      <c r="B44" s="53"/>
       <c r="C44" s="68"/>
       <c r="D44" s="67"/>
       <c r="E44" s="64"/>
@@ -3693,9 +3722,7 @@
       <c r="I44" s="68"/>
       <c r="J44" s="68"/>
       <c r="K44" s="64"/>
-      <c r="L44" t="s" s="69">
-        <v>83</v>
-      </c>
+      <c r="L44" s="69"/>
       <c r="M44" s="64"/>
       <c r="N44" s="64"/>
       <c r="O44" s="64"/>
@@ -3712,22 +3739,28 @@
       <c r="Z44" s="15"/>
       <c r="AA44" s="15"/>
     </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" t="s" s="65">
-        <v>43</v>
+    <row r="45" ht="30.75" customHeight="1">
+      <c r="A45" t="s" s="70">
+        <v>20</v>
       </c>
-      <c r="B45" s="53"/>
-      <c r="C45" s="68"/>
-      <c r="D45" s="67"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="68"/>
-      <c r="H45" s="64"/>
-      <c r="I45" s="68"/>
-      <c r="J45" s="68"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="69"/>
-      <c r="M45" s="64"/>
+      <c r="B45" t="s" s="70">
+        <v>87</v>
+      </c>
+      <c r="C45" t="s" s="71">
+        <v>88</v>
+      </c>
+      <c r="D45" s="72"/>
+      <c r="E45" s="72"/>
+      <c r="F45" t="s" s="70">
+        <v>35</v>
+      </c>
+      <c r="G45" s="73"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="72"/>
+      <c r="L45" s="73"/>
+      <c r="M45" s="74"/>
       <c r="N45" s="64"/>
       <c r="O45" s="64"/>
       <c r="P45" s="14"/>
@@ -3743,31 +3776,31 @@
       <c r="Z45" s="15"/>
       <c r="AA45" s="15"/>
     </row>
-    <row r="46" ht="30.75" customHeight="1">
-      <c r="A46" t="s" s="70">
+    <row r="46" ht="15.75" customHeight="1">
+      <c r="A46" t="s" s="75">
         <v>20</v>
       </c>
-      <c r="B46" t="s" s="70">
-        <v>84</v>
+      <c r="B46" t="s" s="75">
+        <v>89</v>
       </c>
-      <c r="C46" t="s" s="71">
-        <v>85</v>
+      <c r="C46" t="s" s="76">
+        <v>90</v>
       </c>
-      <c r="D46" s="72"/>
-      <c r="E46" s="72"/>
-      <c r="F46" t="s" s="70">
+      <c r="D46" s="77"/>
+      <c r="E46" s="77"/>
+      <c r="F46" t="s" s="75">
         <v>35</v>
       </c>
-      <c r="G46" s="73"/>
-      <c r="H46" s="72"/>
-      <c r="I46" s="73"/>
-      <c r="J46" s="73"/>
-      <c r="K46" s="72"/>
-      <c r="L46" s="73"/>
-      <c r="M46" s="74"/>
-      <c r="N46" s="64"/>
-      <c r="O46" s="64"/>
-      <c r="P46" s="14"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="77"/>
+      <c r="I46" s="78"/>
+      <c r="J46" s="78"/>
+      <c r="K46" s="77"/>
+      <c r="L46" s="78"/>
+      <c r="M46" s="77"/>
+      <c r="N46" s="79"/>
+      <c r="O46" s="79"/>
+      <c r="P46" s="15"/>
       <c r="Q46" s="15"/>
       <c r="R46" s="15"/>
       <c r="S46" s="15"/>
@@ -3782,28 +3815,28 @@
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" t="s" s="75">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s" s="75">
-        <v>86</v>
+        <v>1</v>
       </c>
-      <c r="C47" t="s" s="76">
-        <v>87</v>
+      <c r="C47" s="78"/>
+      <c r="D47" s="77"/>
+      <c r="E47" t="s" s="75">
+        <v>23</v>
       </c>
-      <c r="D47" s="77"/>
-      <c r="E47" s="77"/>
-      <c r="F47" t="s" s="75">
-        <v>35</v>
-      </c>
+      <c r="F47" s="77"/>
       <c r="G47" s="78"/>
       <c r="H47" s="77"/>
       <c r="I47" s="78"/>
       <c r="J47" s="78"/>
       <c r="K47" s="77"/>
-      <c r="L47" s="78"/>
+      <c r="L47" t="s" s="76">
+        <v>91</v>
+      </c>
       <c r="M47" s="77"/>
-      <c r="N47" s="79"/>
-      <c r="O47" s="79"/>
+      <c r="N47" s="80"/>
+      <c r="O47" s="80"/>
       <c r="P47" s="15"/>
       <c r="Q47" s="15"/>
       <c r="R47" s="15"/>
@@ -3817,30 +3850,36 @@
       <c r="Z47" s="15"/>
       <c r="AA47" s="15"/>
     </row>
-    <row r="48" ht="15.75" customHeight="1">
+    <row r="48" ht="12.75" customHeight="1">
       <c r="A48" t="s" s="75">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="B48" t="s" s="75">
-        <v>1</v>
+        <v>92</v>
       </c>
-      <c r="C48" s="78"/>
+      <c r="C48" t="s" s="76">
+        <v>93</v>
+      </c>
       <c r="D48" s="77"/>
       <c r="E48" t="s" s="75">
-        <v>23</v>
+        <v>94</v>
       </c>
-      <c r="F48" s="77"/>
+      <c r="F48" t="s" s="75">
+        <v>35</v>
+      </c>
       <c r="G48" s="78"/>
-      <c r="H48" s="77"/>
+      <c r="H48" t="s" s="75">
+        <v>95</v>
+      </c>
       <c r="I48" s="78"/>
-      <c r="J48" s="78"/>
+      <c r="J48" t="s" s="76">
+        <v>96</v>
+      </c>
       <c r="K48" s="77"/>
-      <c r="L48" t="s" s="76">
-        <v>88</v>
-      </c>
+      <c r="L48" s="78"/>
       <c r="M48" s="77"/>
-      <c r="N48" s="80"/>
-      <c r="O48" s="80"/>
+      <c r="N48" s="81"/>
+      <c r="O48" s="81"/>
       <c r="P48" s="15"/>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
@@ -3854,37 +3893,31 @@
       <c r="Z48" s="15"/>
       <c r="AA48" s="15"/>
     </row>
-    <row r="49" ht="12.75" customHeight="1">
+    <row r="49" ht="30.75" customHeight="1">
       <c r="A49" t="s" s="75">
         <v>20</v>
       </c>
       <c r="B49" t="s" s="75">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="C49" t="s" s="76">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="D49" s="77"/>
-      <c r="E49" t="s" s="75">
-        <v>91</v>
-      </c>
+      <c r="E49" s="77"/>
       <c r="F49" t="s" s="75">
         <v>35</v>
       </c>
       <c r="G49" s="78"/>
-      <c r="H49" t="s" s="75">
-        <v>92</v>
-      </c>
+      <c r="H49" s="77"/>
       <c r="I49" s="78"/>
-      <c r="J49" t="s" s="76">
-        <v>93</v>
-      </c>
+      <c r="J49" s="78"/>
       <c r="K49" s="77"/>
       <c r="L49" s="78"/>
-      <c r="M49" s="77"/>
-      <c r="N49" s="81"/>
-      <c r="O49" s="81"/>
-      <c r="P49" s="15"/>
+      <c r="M49" s="82"/>
+      <c r="N49" s="68"/>
+      <c r="O49" s="68"/>
+      <c r="P49" s="14"/>
       <c r="Q49" s="15"/>
       <c r="R49" s="15"/>
       <c r="S49" s="15"/>
@@ -3897,22 +3930,24 @@
       <c r="Z49" s="15"/>
       <c r="AA49" s="15"/>
     </row>
-    <row r="50" ht="30.75" customHeight="1">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" t="s" s="75">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="B50" t="s" s="75">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="C50" t="s" s="76">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="D50" s="77"/>
       <c r="E50" s="77"/>
       <c r="F50" t="s" s="75">
         <v>35</v>
       </c>
-      <c r="G50" s="78"/>
+      <c r="G50" t="s" s="76">
+        <v>102</v>
+      </c>
       <c r="H50" s="77"/>
       <c r="I50" s="78"/>
       <c r="J50" s="78"/>
@@ -3934,27 +3969,33 @@
       <c r="Z50" s="15"/>
       <c r="AA50" s="15"/>
     </row>
-    <row r="51" ht="15.75" customHeight="1">
+    <row r="51" ht="26.25" customHeight="1">
       <c r="A51" t="s" s="75">
-        <v>96</v>
+        <v>20</v>
       </c>
       <c r="B51" t="s" s="75">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="C51" t="s" s="76">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D51" s="77"/>
-      <c r="E51" s="77"/>
+      <c r="E51" t="s" s="75">
+        <v>94</v>
+      </c>
       <c r="F51" t="s" s="75">
         <v>35</v>
       </c>
-      <c r="G51" t="s" s="76">
-        <v>99</v>
+      <c r="G51" s="78"/>
+      <c r="H51" t="s" s="75">
+        <v>104</v>
       </c>
-      <c r="H51" s="77"/>
-      <c r="I51" s="78"/>
-      <c r="J51" s="78"/>
+      <c r="I51" t="s" s="76">
+        <v>105</v>
+      </c>
+      <c r="J51" t="s" s="76">
+        <v>106</v>
+      </c>
       <c r="K51" s="77"/>
       <c r="L51" s="78"/>
       <c r="M51" s="82"/>
@@ -3973,38 +4014,38 @@
       <c r="Z51" s="15"/>
       <c r="AA51" s="15"/>
     </row>
-    <row r="52" ht="26.25" customHeight="1">
+    <row r="52" ht="12.75" customHeight="1">
       <c r="A52" t="s" s="75">
         <v>20</v>
       </c>
       <c r="B52" t="s" s="75">
-        <v>38</v>
+        <v>107</v>
       </c>
       <c r="C52" t="s" s="76">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="D52" s="77"/>
       <c r="E52" t="s" s="75">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F52" t="s" s="75">
-        <v>35</v>
+        <v>109</v>
       </c>
       <c r="G52" s="78"/>
       <c r="H52" t="s" s="75">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="I52" t="s" s="76">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="J52" t="s" s="76">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="K52" s="77"/>
       <c r="L52" s="78"/>
       <c r="M52" s="82"/>
-      <c r="N52" s="68"/>
-      <c r="O52" s="68"/>
+      <c r="N52" s="54"/>
+      <c r="O52" s="54"/>
       <c r="P52" s="14"/>
       <c r="Q52" s="15"/>
       <c r="R52" s="15"/>
@@ -4019,38 +4060,22 @@
       <c r="AA52" s="15"/>
     </row>
     <row r="53" ht="12.75" customHeight="1">
-      <c r="A53" t="s" s="75">
-        <v>20</v>
-      </c>
-      <c r="B53" t="s" s="75">
-        <v>104</v>
-      </c>
-      <c r="C53" t="s" s="76">
-        <v>105</v>
-      </c>
+      <c r="A53" s="77"/>
+      <c r="B53" s="77"/>
+      <c r="C53" s="78"/>
       <c r="D53" s="77"/>
-      <c r="E53" t="s" s="75">
-        <v>91</v>
-      </c>
-      <c r="F53" t="s" s="75">
-        <v>106</v>
-      </c>
+      <c r="E53" s="77"/>
+      <c r="F53" s="77"/>
       <c r="G53" s="78"/>
-      <c r="H53" t="s" s="75">
-        <v>101</v>
-      </c>
-      <c r="I53" t="s" s="76">
-        <v>102</v>
-      </c>
-      <c r="J53" t="s" s="76">
-        <v>103</v>
-      </c>
+      <c r="H53" s="77"/>
+      <c r="I53" s="78"/>
+      <c r="J53" s="78"/>
       <c r="K53" s="77"/>
       <c r="L53" s="78"/>
-      <c r="M53" s="82"/>
-      <c r="N53" s="54"/>
-      <c r="O53" s="54"/>
-      <c r="P53" s="14"/>
+      <c r="M53" s="77"/>
+      <c r="N53" s="83"/>
+      <c r="O53" s="83"/>
+      <c r="P53" s="15"/>
       <c r="Q53" s="15"/>
       <c r="R53" s="15"/>
       <c r="S53" s="15"/>
@@ -4064,21 +4089,31 @@
       <c r="AA53" s="15"/>
     </row>
     <row r="54" ht="12.75" customHeight="1">
-      <c r="A54" s="77"/>
-      <c r="B54" s="77"/>
-      <c r="C54" s="78"/>
+      <c r="A54" t="s" s="75">
+        <v>110</v>
+      </c>
+      <c r="B54" t="s" s="75">
+        <v>111</v>
+      </c>
+      <c r="C54" t="s" s="76">
+        <v>112</v>
+      </c>
       <c r="D54" s="77"/>
       <c r="E54" s="77"/>
-      <c r="F54" s="77"/>
+      <c r="F54" t="s" s="75">
+        <v>35</v>
+      </c>
       <c r="G54" s="78"/>
-      <c r="H54" s="77"/>
+      <c r="H54" t="s" s="75">
+        <v>113</v>
+      </c>
       <c r="I54" s="78"/>
       <c r="J54" s="78"/>
       <c r="K54" s="77"/>
       <c r="L54" s="78"/>
       <c r="M54" s="77"/>
-      <c r="N54" s="83"/>
-      <c r="O54" s="83"/>
+      <c r="N54" s="15"/>
+      <c r="O54" s="15"/>
       <c r="P54" s="15"/>
       <c r="Q54" s="15"/>
       <c r="R54" s="15"/>
@@ -4094,27 +4129,27 @@
     </row>
     <row r="55" ht="12.75" customHeight="1">
       <c r="A55" t="s" s="75">
-        <v>107</v>
+        <v>44</v>
       </c>
       <c r="B55" t="s" s="75">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="C55" t="s" s="76">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="D55" s="77"/>
-      <c r="E55" s="77"/>
-      <c r="F55" t="s" s="75">
-        <v>35</v>
+      <c r="E55" t="s" s="75">
+        <v>23</v>
       </c>
+      <c r="F55" s="75"/>
       <c r="G55" s="78"/>
-      <c r="H55" t="s" s="75">
-        <v>109</v>
-      </c>
+      <c r="H55" s="75"/>
       <c r="I55" s="78"/>
       <c r="J55" s="78"/>
       <c r="K55" s="77"/>
-      <c r="L55" s="78"/>
+      <c r="L55" t="s" s="76">
+        <v>116</v>
+      </c>
       <c r="M55" s="77"/>
       <c r="N55" s="15"/>
       <c r="O55" s="15"/>
@@ -32261,7 +32296,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" t="s" s="87">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s" s="87">
         <v>1</v>
@@ -32379,13 +32414,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" t="s" s="90">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="B5" t="s" s="90">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="C5" t="s" s="90">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
@@ -32413,13 +32448,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" t="s" s="90">
-        <v>53</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s" s="90">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="C6" t="s" s="90">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="D6" s="89"/>
       <c r="E6" s="89"/>
@@ -32615,13 +32650,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" t="s" s="90">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B13" t="s" s="90">
         <v>35</v>
       </c>
       <c r="C13" t="s" s="90">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
@@ -32649,13 +32684,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" t="s" s="90">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B14" t="s" s="90">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s" s="90">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
@@ -60036,19 +60071,19 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="92">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B1" t="s" s="92">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C1" t="s" s="92">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D1" t="s" s="92">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="E1" t="s" s="92">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="F1" s="92"/>
       <c r="G1" s="92"/>
@@ -60063,19 +60098,19 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="93">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B2" t="s" s="94">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C2" s="95">
         <v>43900</v>
       </c>
       <c r="D2" t="s" s="94">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="E2" t="s" s="94">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="F2" s="96"/>
       <c r="G2" s="96"/>

</xml_diff>

<commit_message>
feat: add temporary telegram id field for (#200)
</commit_message>
<xml_diff>
--- a/itech-malawi/forms/app/enroll.xlsx
+++ b/itech-malawi/forms/app/enroll.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
   <si>
     <t>type</t>
   </si>
@@ -364,6 +364,15 @@
   </si>
   <si>
     <t>if(selected(${language_preference}, ’english’), ‘eng’, ‘nya’)</t>
+  </si>
+  <si>
+    <t>telegram_id</t>
+  </si>
+  <si>
+    <t>Telegram ID</t>
+  </si>
+  <si>
+    <t>This is for test purpose only</t>
   </si>
   <si>
     <t>list_name</t>
@@ -2135,7 +2144,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA1024"/>
+  <dimension ref="A1:AA1025"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2152,7 +2161,7 @@
     <col min="9" max="9" width="30.3516" style="1" customWidth="1"/>
     <col min="10" max="10" width="27.3516" style="1" customWidth="1"/>
     <col min="11" max="11" width="13.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="49.5859" style="1" customWidth="1"/>
+    <col min="12" max="12" width="49.6719" style="1" customWidth="1"/>
     <col min="13" max="13" width="17.8516" style="1" customWidth="1"/>
     <col min="14" max="14" width="20.8516" style="1" customWidth="1"/>
     <col min="15" max="15" width="13.8516" style="1" customWidth="1"/>
@@ -4167,21 +4176,29 @@
       <c r="AA55" s="15"/>
     </row>
     <row r="56" ht="12.75" customHeight="1">
-      <c r="A56" t="s" s="84">
-        <v>43</v>
+      <c r="A56" t="s" s="75">
+        <v>20</v>
       </c>
-      <c r="B56" s="15"/>
-      <c r="C56" s="85"/>
-      <c r="D56" s="15"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="15"/>
-      <c r="G56" s="85"/>
-      <c r="H56" s="15"/>
-      <c r="I56" s="85"/>
-      <c r="J56" s="85"/>
-      <c r="K56" s="15"/>
-      <c r="L56" s="85"/>
-      <c r="M56" s="15"/>
+      <c r="B56" t="s" s="75">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s" s="76">
+        <v>118</v>
+      </c>
+      <c r="D56" s="77"/>
+      <c r="E56" s="75"/>
+      <c r="F56" t="s" s="75">
+        <v>109</v>
+      </c>
+      <c r="G56" s="78"/>
+      <c r="H56" s="75"/>
+      <c r="I56" s="78"/>
+      <c r="J56" t="s" s="76">
+        <v>119</v>
+      </c>
+      <c r="K56" s="77"/>
+      <c r="L56" s="76"/>
+      <c r="M56" s="77"/>
       <c r="N56" s="15"/>
       <c r="O56" s="15"/>
       <c r="P56" s="15"/>
@@ -4198,7 +4215,9 @@
       <c r="AA56" s="15"/>
     </row>
     <row r="57" ht="12.75" customHeight="1">
-      <c r="A57" s="15"/>
+      <c r="A57" t="s" s="84">
+        <v>43</v>
+      </c>
       <c r="B57" s="15"/>
       <c r="C57" s="85"/>
       <c r="D57" s="15"/>
@@ -9301,7 +9320,7 @@
       <c r="Z232" s="15"/>
       <c r="AA232" s="15"/>
     </row>
-    <row r="233" ht="15.75" customHeight="1">
+    <row r="233" ht="12.75" customHeight="1">
       <c r="A233" s="15"/>
       <c r="B233" s="15"/>
       <c r="C233" s="85"/>
@@ -31776,7 +31795,7 @@
       <c r="Z1007" s="15"/>
       <c r="AA1007" s="15"/>
     </row>
-    <row r="1008" ht="15" customHeight="1">
+    <row r="1008" ht="15.75" customHeight="1">
       <c r="A1008" s="15"/>
       <c r="B1008" s="15"/>
       <c r="C1008" s="85"/>
@@ -31789,21 +31808,21 @@
       <c r="J1008" s="85"/>
       <c r="K1008" s="15"/>
       <c r="L1008" s="85"/>
-      <c r="M1008" s="77"/>
-      <c r="N1008" s="77"/>
-      <c r="O1008" s="77"/>
-      <c r="P1008" s="77"/>
-      <c r="Q1008" s="77"/>
-      <c r="R1008" s="77"/>
-      <c r="S1008" s="77"/>
-      <c r="T1008" s="77"/>
-      <c r="U1008" s="77"/>
-      <c r="V1008" s="77"/>
-      <c r="W1008" s="77"/>
-      <c r="X1008" s="77"/>
-      <c r="Y1008" s="77"/>
-      <c r="Z1008" s="77"/>
-      <c r="AA1008" s="77"/>
+      <c r="M1008" s="15"/>
+      <c r="N1008" s="15"/>
+      <c r="O1008" s="15"/>
+      <c r="P1008" s="15"/>
+      <c r="Q1008" s="15"/>
+      <c r="R1008" s="15"/>
+      <c r="S1008" s="15"/>
+      <c r="T1008" s="15"/>
+      <c r="U1008" s="15"/>
+      <c r="V1008" s="15"/>
+      <c r="W1008" s="15"/>
+      <c r="X1008" s="15"/>
+      <c r="Y1008" s="15"/>
+      <c r="Z1008" s="15"/>
+      <c r="AA1008" s="15"/>
     </row>
     <row r="1009" ht="15" customHeight="1">
       <c r="A1009" s="15"/>
@@ -32269,6 +32288,35 @@
       <c r="Z1024" s="77"/>
       <c r="AA1024" s="77"/>
     </row>
+    <row r="1025" ht="15" customHeight="1">
+      <c r="A1025" s="15"/>
+      <c r="B1025" s="15"/>
+      <c r="C1025" s="85"/>
+      <c r="D1025" s="15"/>
+      <c r="E1025" s="15"/>
+      <c r="F1025" s="15"/>
+      <c r="G1025" s="85"/>
+      <c r="H1025" s="15"/>
+      <c r="I1025" s="85"/>
+      <c r="J1025" s="85"/>
+      <c r="K1025" s="15"/>
+      <c r="L1025" s="85"/>
+      <c r="M1025" s="77"/>
+      <c r="N1025" s="77"/>
+      <c r="O1025" s="77"/>
+      <c r="P1025" s="77"/>
+      <c r="Q1025" s="77"/>
+      <c r="R1025" s="77"/>
+      <c r="S1025" s="77"/>
+      <c r="T1025" s="77"/>
+      <c r="U1025" s="77"/>
+      <c r="V1025" s="77"/>
+      <c r="W1025" s="77"/>
+      <c r="X1025" s="77"/>
+      <c r="Y1025" s="77"/>
+      <c r="Z1025" s="77"/>
+      <c r="AA1025" s="77"/>
+    </row>
   </sheetData>
   <pageMargins left="0.747917" right="0.747917" top="0.984028" bottom="0.984028" header="0" footer="0"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -32296,7 +32344,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" t="s" s="87">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B1" t="s" s="87">
         <v>1</v>
@@ -32417,10 +32465,10 @@
         <v>111</v>
       </c>
       <c r="B5" t="s" s="90">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="C5" t="s" s="90">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="D5" s="89"/>
       <c r="E5" s="89"/>
@@ -32451,10 +32499,10 @@
         <v>111</v>
       </c>
       <c r="B6" t="s" s="90">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C6" t="s" s="90">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D6" s="89"/>
       <c r="E6" s="89"/>
@@ -32650,13 +32698,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" t="s" s="90">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s" s="90">
         <v>35</v>
       </c>
       <c r="C13" t="s" s="90">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D13" s="89"/>
       <c r="E13" s="89"/>
@@ -32684,13 +32732,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" t="s" s="90">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s" s="90">
         <v>109</v>
       </c>
       <c r="C14" t="s" s="90">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="D14" s="89"/>
       <c r="E14" s="89"/>
@@ -60071,19 +60119,19 @@
   <sheetData>
     <row r="1" ht="18" customHeight="1">
       <c r="A1" t="s" s="92">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="B1" t="s" s="92">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C1" t="s" s="92">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s" s="92">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="E1" t="s" s="92">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="F1" s="92"/>
       <c r="G1" s="92"/>
@@ -60098,19 +60146,19 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" t="s" s="93">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B2" t="s" s="94">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="C2" s="95">
         <v>43900</v>
       </c>
       <c r="D2" t="s" s="94">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="E2" t="s" s="94">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="F2" s="96"/>
       <c r="G2" s="96"/>

</xml_diff>